<commit_message>
- added food_direction to domain.yml
</commit_message>
<xml_diff>
--- a/restaurantData/Restaurant_DB.xlsx
+++ b/restaurantData/Restaurant_DB.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/normanschmickler/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13C8CC3D-25B3-8445-AAA5-A35A5BF72C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{04757E8A-D0ED-6E4E-A43C-351DE8677651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="40960" windowHeight="23040" xr2:uid="{106D1393-4DC9-4DB8-A467-A49FAB233FCB}"/>
+    <workbookView xWindow="20" yWindow="520" windowWidth="28800" windowHeight="16460" xr2:uid="{106D1393-4DC9-4DB8-A467-A49FAB233FCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Restaurants" sheetId="3" r:id="rId1"/>
     <sheet name="Gerichte" sheetId="1" r:id="rId2"/>
-    <sheet name="Getränke" sheetId="2" r:id="rId3"/>
-    <sheet name="Besonderheiten" sheetId="4" r:id="rId4"/>
-    <sheet name="Allergene" sheetId="7" r:id="rId5"/>
-    <sheet name="Notizen" sheetId="5" r:id="rId6"/>
-    <sheet name="Kundendetails " sheetId="6" r:id="rId7"/>
+    <sheet name="Kategorie" sheetId="9" r:id="rId3"/>
+    <sheet name="Zutaten" sheetId="8" r:id="rId4"/>
+    <sheet name="Getränke" sheetId="2" r:id="rId5"/>
+    <sheet name="Besonderheiten" sheetId="4" r:id="rId6"/>
+    <sheet name="Allergene" sheetId="7" r:id="rId7"/>
+    <sheet name="Notizen" sheetId="5" r:id="rId8"/>
+    <sheet name="Kundendetails " sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1298" uniqueCount="861">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1318" uniqueCount="874">
   <si>
     <t>Restaurant_ID</t>
   </si>
@@ -1246,9 +1248,6 @@
     <t>https://th.bing.com/th/id/OIP.0V3y_iSEDExdJhyrmKVBNgHaGc?pid=ImgDet&amp;rs=1</t>
   </si>
   <si>
-    <t>Pizza, Käse, Mozarella, Tomate, Wurst, Salami</t>
-  </si>
-  <si>
     <t>PIZZA VEGATARIANA</t>
   </si>
   <si>
@@ -2651,6 +2650,48 @@
   </si>
   <si>
     <t>durchgehend geöffnet</t>
+  </si>
+  <si>
+    <t>Zutaten_ID</t>
+  </si>
+  <si>
+    <t>Kartoffel</t>
+  </si>
+  <si>
+    <t>Kategorie_ID</t>
+  </si>
+  <si>
+    <t>Protein</t>
+  </si>
+  <si>
+    <t>Fleisch</t>
+  </si>
+  <si>
+    <t>Carbs</t>
+  </si>
+  <si>
+    <t>Bitte wähle deine Grundlage</t>
+  </si>
+  <si>
+    <t>Käse, Mozarella, Tomate, Fleisch, Salami, Weizen</t>
+  </si>
+  <si>
+    <t>Beispiel</t>
+  </si>
+  <si>
+    <t>Kartoffel, reis, weizen, nudel, linse</t>
+  </si>
+  <si>
+    <t>Linse, Tofu, Fleisch, Salami, Bohne</t>
+  </si>
+  <si>
+    <t>Green/Extra</t>
+  </si>
+  <si>
+    <t>Salat, Erdnuss, Basilikum, Nüsse, Käse, Gemüse, Paprika</t>
+  </si>
+  <si>
+    <t>Extra button für kein carb, protein oder green</t>
   </si>
 </sst>
 </file>
@@ -2842,7 +2883,7 @@
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="53">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2914,6 +2955,39 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3039,50 +3113,75 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{80FDB988-FCAC-8D44-99D6-7DFF600B82CE}" name="Tabelle1" displayName="Tabelle1" ref="A1:N19" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{80FDB988-FCAC-8D44-99D6-7DFF600B82CE}" name="Tabelle1" displayName="Tabelle1" ref="A1:N19" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
   <autoFilter ref="A1:N19" xr:uid="{80FDB988-FCAC-8D44-99D6-7DFF600B82CE}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{55A32A4D-2FF6-6A4E-815C-A2710FF99FDF}" name="Restaurant_ID" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{6E4C25BB-32A3-7B4B-A9AC-13B82E8BF2F1}" name="Restaurant_Name" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{128C870C-3194-E84E-83F4-79DB4C4E7BA0}" name="Kategorie" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{3408C74D-0A76-5F40-BD7D-CD57DAC13688}" name="Beschreibung" dataDxfId="36"/>
-    <tableColumn id="13" xr3:uid="{09E09216-F076-EF47-B03C-46543813370D}" name="Öffnet_Mittags" dataDxfId="35"/>
-    <tableColumn id="12" xr3:uid="{37FAB9EF-BE2C-6549-B0B2-8C7258215DF1}" name="Schließt_Mittags" dataDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{A3BAD815-DDD1-584F-913C-BEBC1E18A73D}" name="Öffnet_Abends" dataDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{FD4D8756-8444-EE4A-A5DD-41872DCC4B47}" name="Schließt_Abends" dataDxfId="32"/>
-    <tableColumn id="7" xr3:uid="{A4AB5AB3-CC69-2346-87DA-103B4479D1F7}" name="Öffnungstage" dataDxfId="31"/>
-    <tableColumn id="8" xr3:uid="{4EB62772-A5B6-3447-BBDA-4F9E1D531970}" name="Preiskategorie" dataDxfId="30"/>
-    <tableColumn id="9" xr3:uid="{5190CBEF-FD7B-A04E-84EE-B3EED4FD94EA}" name="Bewertung" dataDxfId="29"/>
-    <tableColumn id="10" xr3:uid="{05D6B2BC-6F3F-0F4D-81D9-48B283052F62}" name="Adresse" dataDxfId="28"/>
-    <tableColumn id="15" xr3:uid="{6C452FD0-68CB-574B-AEFC-15A45D09A146}" name="Telefon" dataDxfId="27"/>
-    <tableColumn id="14" xr3:uid="{F036DC08-DE13-9E4C-8BAB-A155392C2417}" name="Website" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{55A32A4D-2FF6-6A4E-815C-A2710FF99FDF}" name="Restaurant_ID" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{6E4C25BB-32A3-7B4B-A9AC-13B82E8BF2F1}" name="Restaurant_Name" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{128C870C-3194-E84E-83F4-79DB4C4E7BA0}" name="Kategorie" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{3408C74D-0A76-5F40-BD7D-CD57DAC13688}" name="Beschreibung" dataDxfId="47"/>
+    <tableColumn id="13" xr3:uid="{09E09216-F076-EF47-B03C-46543813370D}" name="Öffnet_Mittags" dataDxfId="46"/>
+    <tableColumn id="12" xr3:uid="{37FAB9EF-BE2C-6549-B0B2-8C7258215DF1}" name="Schließt_Mittags" dataDxfId="45"/>
+    <tableColumn id="5" xr3:uid="{A3BAD815-DDD1-584F-913C-BEBC1E18A73D}" name="Öffnet_Abends" dataDxfId="44"/>
+    <tableColumn id="6" xr3:uid="{FD4D8756-8444-EE4A-A5DD-41872DCC4B47}" name="Schließt_Abends" dataDxfId="43"/>
+    <tableColumn id="7" xr3:uid="{A4AB5AB3-CC69-2346-87DA-103B4479D1F7}" name="Öffnungstage" dataDxfId="42"/>
+    <tableColumn id="8" xr3:uid="{4EB62772-A5B6-3447-BBDA-4F9E1D531970}" name="Preiskategorie" dataDxfId="41"/>
+    <tableColumn id="9" xr3:uid="{5190CBEF-FD7B-A04E-84EE-B3EED4FD94EA}" name="Bewertung" dataDxfId="40"/>
+    <tableColumn id="10" xr3:uid="{05D6B2BC-6F3F-0F4D-81D9-48B283052F62}" name="Adresse" dataDxfId="39"/>
+    <tableColumn id="15" xr3:uid="{6C452FD0-68CB-574B-AEFC-15A45D09A146}" name="Telefon" dataDxfId="38"/>
+    <tableColumn id="14" xr3:uid="{F036DC08-DE13-9E4C-8BAB-A155392C2417}" name="Website" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B3CAD1EC-7155-BE41-89CD-997BF4A0D027}" name="Tabelle3" displayName="Tabelle3" ref="A1:L101" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B3CAD1EC-7155-BE41-89CD-997BF4A0D027}" name="Tabelle3" displayName="Tabelle3" ref="A1:L101" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
   <autoFilter ref="A1:L101" xr:uid="{B3CAD1EC-7155-BE41-89CD-997BF4A0D027}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{CFA5AF43-D759-BF47-A92B-03D5569460AD}" name="Gericht_ID" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{CA124AC5-0B98-0D48-B262-D3055FC1D666}" name="Kategorie" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{8E8DA039-2403-E042-B872-C45B85971D05}" name="Name" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{FCCDA6D9-059C-BA49-BCEB-8DCE30979128}" name="Preis" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{B87CBEA8-0855-D048-B466-05B1A4BA8431}" name="veg" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{15116D70-7FB7-7B41-9E2D-57E36F08539B}" name="Besonderheit" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{6149EE81-7057-D34A-9583-8D862C7228E3}" name="Allergene" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{84779147-51E7-DE4B-B3B9-99F094548C15}" name="Gang" dataDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{6B937401-4F11-B44D-BDD9-8084A3AEC23F}" name="Beschreibung" dataDxfId="15"/>
-    <tableColumn id="10" xr3:uid="{C5B87709-C104-334F-B54D-D9AE69ADED8C}" name="Bild" dataDxfId="14"/>
-    <tableColumn id="11" xr3:uid="{EEF2CE40-FEF7-6D41-BF14-43F7949A9AEB}" name="Zutaten" dataDxfId="13"/>
-    <tableColumn id="12" xr3:uid="{484E0797-2CF8-4A6F-98D0-B629421F46E3}" name="FK_Restaurant" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{CFA5AF43-D759-BF47-A92B-03D5569460AD}" name="Gericht_ID" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{CA124AC5-0B98-0D48-B262-D3055FC1D666}" name="Kategorie" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{8E8DA039-2403-E042-B872-C45B85971D05}" name="Name" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{FCCDA6D9-059C-BA49-BCEB-8DCE30979128}" name="Preis" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{B87CBEA8-0855-D048-B466-05B1A4BA8431}" name="veg" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{15116D70-7FB7-7B41-9E2D-57E36F08539B}" name="Besonderheit" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{6149EE81-7057-D34A-9583-8D862C7228E3}" name="Allergene" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{84779147-51E7-DE4B-B3B9-99F094548C15}" name="Gang" dataDxfId="27"/>
+    <tableColumn id="9" xr3:uid="{6B937401-4F11-B44D-BDD9-8084A3AEC23F}" name="Beschreibung" dataDxfId="26"/>
+    <tableColumn id="10" xr3:uid="{C5B87709-C104-334F-B54D-D9AE69ADED8C}" name="Bild" dataDxfId="25"/>
+    <tableColumn id="11" xr3:uid="{EEF2CE40-FEF7-6D41-BF14-43F7949A9AEB}" name="Zutaten" dataDxfId="24"/>
+    <tableColumn id="12" xr3:uid="{484E0797-2CF8-4A6F-98D0-B629421F46E3}" name="FK_Restaurant" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9B6555A2-C786-7B40-A974-B41D15183573}" name="Tabelle57" displayName="Tabelle57" ref="A1:D14" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+  <autoFilter ref="A1:D14" xr:uid="{B0AE1103-1826-F645-B10B-83B5258131B7}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{274AA7BB-D327-9F4B-98F2-A1EDC7D7A378}" name="Kategorie_ID" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{5DF70DE5-ECFE-514A-AAE4-0AD449EE91F9}" name="Name" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{A66ACFD1-1291-8D48-8033-43AA0CD9395B}" name="Beschreibung" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{BD6C68A9-E579-3348-8F25-A2A208F21A06}" name="Beispiel" dataDxfId="17"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B0AE1103-1826-F645-B10B-83B5258131B7}" name="Tabelle5" displayName="Tabelle5" ref="A1:C15" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="A1:C15" xr:uid="{B0AE1103-1826-F645-B10B-83B5258131B7}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{769D3B1F-BDD9-9842-8D20-AF6022CE7F40}" name="Zutaten_ID" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{A2F4A89D-E730-394F-B34D-6DEF77C752E3}" name="Name" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{49E9EC0A-978D-EF48-B509-9FD05461693B}" name="Kategorie" dataDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8EE87F00-AE3F-4A3F-8E64-0260D4DB755C}" name="Tabelle7" displayName="Tabelle7" ref="A1:E53" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10">
   <autoFilter ref="A1:E53" xr:uid="{8EE87F00-AE3F-4A3F-8E64-0260D4DB755C}"/>
   <tableColumns count="5">
@@ -3096,7 +3195,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{12FC1B5A-ABE0-4C4C-9FD4-80616E6F351F}" name="Tabelle2" displayName="Tabelle2" ref="A1:B49" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:B49" xr:uid="{12FC1B5A-ABE0-4C4C-9FD4-80616E6F351F}"/>
   <tableColumns count="2">
@@ -3107,7 +3206,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6F512E60-FBCC-9F46-897C-F96C5CA98126}" name="Tabelle25" displayName="Tabelle25" ref="A1:C24" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A1:C24" xr:uid="{12FC1B5A-ABE0-4C4C-9FD4-80616E6F351F}"/>
   <tableColumns count="3">
@@ -3418,7 +3517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{721D09D1-6061-4240-90BA-F30DB895FBD6}">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="97" workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
@@ -3593,10 +3692,10 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="H4" s="5">
         <v>0.9375</v>
@@ -3638,10 +3737,10 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="H5" s="5">
         <v>0.91666666666666663</v>
@@ -3773,10 +3872,10 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="H8" s="5">
         <v>0.9375</v>
@@ -4133,10 +4232,10 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="H16" s="5">
         <v>0.91666666666666663</v>
@@ -4473,8 +4572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EB17E25-B77B-4700-B7C6-1DB9B3E38A2C}">
   <dimension ref="A1:M126"/>
   <sheetViews>
-    <sheetView topLeftCell="A101" zoomScale="140" workbookViewId="0">
-      <selection activeCell="A119" sqref="A119:A126"/>
+    <sheetView topLeftCell="A10" zoomScale="140" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6337,7 +6436,7 @@
         <v>392</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>393</v>
+        <v>867</v>
       </c>
       <c r="L49" s="4">
         <v>17</v>
@@ -6351,7 +6450,7 @@
         <v>229</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D50" s="4">
         <v>10.8</v>
@@ -6360,7 +6459,7 @@
         <v>172</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>287</v>
@@ -6369,13 +6468,13 @@
         <v>136</v>
       </c>
       <c r="I50" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="J50" s="7" t="s">
         <v>396</v>
       </c>
-      <c r="J50" s="7" t="s">
+      <c r="K50" s="4" t="s">
         <v>397</v>
-      </c>
-      <c r="K50" s="4" t="s">
-        <v>398</v>
       </c>
       <c r="L50" s="4">
         <v>17</v>
@@ -6389,16 +6488,16 @@
         <v>229</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D51" s="4">
         <v>12.8</v>
       </c>
       <c r="E51" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="F51" s="4" t="s">
         <v>400</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>401</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>382</v>
@@ -6407,13 +6506,13 @@
         <v>136</v>
       </c>
       <c r="I51" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="J51" s="7" t="s">
         <v>402</v>
       </c>
-      <c r="J51" s="7" t="s">
+      <c r="K51" s="4" t="s">
         <v>403</v>
-      </c>
-      <c r="K51" s="4" t="s">
-        <v>404</v>
       </c>
       <c r="L51" s="4">
         <v>17</v>
@@ -6427,7 +6526,7 @@
         <v>229</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D52" s="4">
         <v>12.8</v>
@@ -6436,7 +6535,7 @@
         <v>319</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>376</v>
@@ -6445,13 +6544,13 @@
         <v>136</v>
       </c>
       <c r="I52" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="J52" s="7" t="s">
         <v>407</v>
       </c>
-      <c r="J52" s="7" t="s">
+      <c r="K52" s="4" t="s">
         <v>408</v>
-      </c>
-      <c r="K52" s="4" t="s">
-        <v>409</v>
       </c>
       <c r="L52" s="4">
         <v>17</v>
@@ -6465,7 +6564,7 @@
         <v>229</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D53" s="4">
         <v>10.8</v>
@@ -6474,22 +6573,22 @@
         <v>172</v>
       </c>
       <c r="F53" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="G53" s="4" t="s">
         <v>411</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>412</v>
       </c>
       <c r="H53" s="4" t="s">
         <v>136</v>
       </c>
       <c r="I53" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="J53" s="7" t="s">
         <v>413</v>
       </c>
-      <c r="J53" s="7" t="s">
+      <c r="K53" s="4" t="s">
         <v>414</v>
-      </c>
-      <c r="K53" s="4" t="s">
-        <v>415</v>
       </c>
       <c r="L53" s="4">
         <v>17</v>
@@ -6503,7 +6602,7 @@
         <v>229</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D54" s="4">
         <v>12.8</v>
@@ -6512,22 +6611,22 @@
         <v>319</v>
       </c>
       <c r="F54" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="G54" s="4" t="s">
         <v>417</v>
-      </c>
-      <c r="G54" s="4" t="s">
-        <v>418</v>
       </c>
       <c r="H54" s="4" t="s">
         <v>136</v>
       </c>
       <c r="I54" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="J54" s="7" t="s">
         <v>419</v>
       </c>
-      <c r="J54" s="7" t="s">
+      <c r="K54" s="4" t="s">
         <v>420</v>
-      </c>
-      <c r="K54" s="4" t="s">
-        <v>421</v>
       </c>
       <c r="L54" s="4">
         <v>17</v>
@@ -6541,7 +6640,7 @@
         <v>229</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D55" s="4">
         <v>10.5</v>
@@ -6550,7 +6649,7 @@
         <v>209</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G55" s="4">
         <v>1</v>
@@ -6559,13 +6658,13 @@
         <v>136</v>
       </c>
       <c r="I55" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="J55" s="7" t="s">
         <v>424</v>
       </c>
-      <c r="J55" s="7" t="s">
+      <c r="K55" s="4" t="s">
         <v>425</v>
-      </c>
-      <c r="K55" s="4" t="s">
-        <v>426</v>
       </c>
       <c r="L55" s="4">
         <v>17</v>
@@ -6579,7 +6678,7 @@
         <v>229</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D56" s="4">
         <v>12.5</v>
@@ -6588,7 +6687,7 @@
         <v>209</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>287</v>
@@ -6597,13 +6696,13 @@
         <v>136</v>
       </c>
       <c r="I56" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="J56" s="7" t="s">
         <v>429</v>
       </c>
-      <c r="J56" s="7" t="s">
+      <c r="K56" s="4" t="s">
         <v>430</v>
-      </c>
-      <c r="K56" s="4" t="s">
-        <v>431</v>
       </c>
       <c r="L56" s="4">
         <v>17</v>
@@ -6617,7 +6716,7 @@
         <v>229</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D57" s="4">
         <v>12.5</v>
@@ -6626,7 +6725,7 @@
         <v>172</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>287</v>
@@ -6635,13 +6734,13 @@
         <v>136</v>
       </c>
       <c r="I57" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="J57" s="7" t="s">
         <v>434</v>
       </c>
-      <c r="J57" s="7" t="s">
+      <c r="K57" s="4" t="s">
         <v>435</v>
-      </c>
-      <c r="K57" s="4" t="s">
-        <v>436</v>
       </c>
       <c r="L57" s="4">
         <v>17</v>
@@ -6655,7 +6754,7 @@
         <v>260</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D58" s="4">
         <v>13.5</v>
@@ -6664,7 +6763,7 @@
         <v>209</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G58" s="4">
         <v>1</v>
@@ -6673,13 +6772,13 @@
         <v>136</v>
       </c>
       <c r="I58" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="J58" s="7" t="s">
         <v>439</v>
       </c>
-      <c r="J58" s="7" t="s">
+      <c r="K58" s="4" t="s">
         <v>440</v>
-      </c>
-      <c r="K58" s="4" t="s">
-        <v>441</v>
       </c>
       <c r="L58" s="4">
         <v>16</v>
@@ -6693,7 +6792,7 @@
         <v>260</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D59" s="4">
         <v>13.5</v>
@@ -6702,20 +6801,20 @@
         <v>209</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="G59" s="4"/>
       <c r="H59" s="4" t="s">
         <v>136</v>
       </c>
       <c r="I59" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="J59" s="7" t="s">
         <v>444</v>
       </c>
-      <c r="J59" s="7" t="s">
+      <c r="K59" s="4" t="s">
         <v>445</v>
-      </c>
-      <c r="K59" s="4" t="s">
-        <v>446</v>
       </c>
       <c r="L59" s="4">
         <v>16</v>
@@ -6729,7 +6828,7 @@
         <v>260</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D60" s="4">
         <v>13.9</v>
@@ -6738,20 +6837,20 @@
         <v>209</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="G60" s="4"/>
       <c r="H60" s="4" t="s">
         <v>136</v>
       </c>
       <c r="I60" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="J60" s="7" t="s">
         <v>448</v>
       </c>
-      <c r="J60" s="7" t="s">
+      <c r="K60" s="4" t="s">
         <v>449</v>
-      </c>
-      <c r="K60" s="4" t="s">
-        <v>450</v>
       </c>
       <c r="L60" s="4">
         <v>16</v>
@@ -6765,7 +6864,7 @@
         <v>260</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D61" s="4">
         <v>13.9</v>
@@ -6774,7 +6873,7 @@
         <v>209</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>344</v>
@@ -6783,13 +6882,13 @@
         <v>136</v>
       </c>
       <c r="I61" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="J61" s="7" t="s">
         <v>453</v>
       </c>
-      <c r="J61" s="7" t="s">
+      <c r="K61" s="4" t="s">
         <v>454</v>
-      </c>
-      <c r="K61" s="4" t="s">
-        <v>455</v>
       </c>
       <c r="L61" s="4">
         <v>16</v>
@@ -6803,7 +6902,7 @@
         <v>260</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D62" s="4">
         <v>14.9</v>
@@ -6812,22 +6911,22 @@
         <v>209</v>
       </c>
       <c r="F62" s="4" t="s">
+        <v>456</v>
+      </c>
+      <c r="G62" s="4" t="s">
         <v>457</v>
-      </c>
-      <c r="G62" s="4" t="s">
-        <v>458</v>
       </c>
       <c r="H62" s="4" t="s">
         <v>136</v>
       </c>
       <c r="I62" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="J62" s="7" t="s">
         <v>459</v>
       </c>
-      <c r="J62" s="7" t="s">
+      <c r="K62" s="4" t="s">
         <v>460</v>
-      </c>
-      <c r="K62" s="4" t="s">
-        <v>461</v>
       </c>
       <c r="L62" s="4">
         <v>16</v>
@@ -6841,7 +6940,7 @@
         <v>260</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D63" s="4">
         <v>16.5</v>
@@ -6850,20 +6949,20 @@
         <v>209</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G63" s="4"/>
       <c r="H63" s="4" t="s">
         <v>136</v>
       </c>
       <c r="I63" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="J63" s="7" t="s">
         <v>463</v>
       </c>
-      <c r="J63" s="7" t="s">
+      <c r="K63" s="4" t="s">
         <v>464</v>
-      </c>
-      <c r="K63" s="4" t="s">
-        <v>465</v>
       </c>
       <c r="L63" s="4">
         <v>16</v>
@@ -6877,7 +6976,7 @@
         <v>280</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D64" s="4">
         <v>8.9</v>
@@ -6886,22 +6985,22 @@
         <v>209</v>
       </c>
       <c r="F64" s="4" t="s">
+        <v>466</v>
+      </c>
+      <c r="G64" s="4" t="s">
         <v>467</v>
-      </c>
-      <c r="G64" s="4" t="s">
-        <v>468</v>
       </c>
       <c r="H64" s="4" t="s">
         <v>136</v>
       </c>
       <c r="I64" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="J64" s="7" t="s">
         <v>469</v>
       </c>
-      <c r="J64" s="7" t="s">
+      <c r="K64" s="4" t="s">
         <v>470</v>
-      </c>
-      <c r="K64" s="4" t="s">
-        <v>471</v>
       </c>
       <c r="L64" s="4">
         <v>15</v>
@@ -6915,7 +7014,7 @@
         <v>280</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D65" s="4">
         <v>9.4</v>
@@ -6924,22 +7023,22 @@
         <v>209</v>
       </c>
       <c r="F65" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="G65" s="4" t="s">
         <v>473</v>
-      </c>
-      <c r="G65" s="4" t="s">
-        <v>474</v>
       </c>
       <c r="H65" s="4" t="s">
         <v>136</v>
       </c>
       <c r="I65" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="J65" s="7" t="s">
         <v>475</v>
       </c>
-      <c r="J65" s="7" t="s">
+      <c r="K65" s="4" t="s">
         <v>476</v>
-      </c>
-      <c r="K65" s="4" t="s">
-        <v>477</v>
       </c>
       <c r="L65" s="4">
         <v>15</v>
@@ -6953,7 +7052,7 @@
         <v>280</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D66" s="4">
         <v>13.4</v>
@@ -6962,22 +7061,22 @@
         <v>209</v>
       </c>
       <c r="F66" s="4" t="s">
+        <v>478</v>
+      </c>
+      <c r="G66" s="4" t="s">
         <v>479</v>
-      </c>
-      <c r="G66" s="4" t="s">
-        <v>480</v>
       </c>
       <c r="H66" s="4" t="s">
         <v>136</v>
       </c>
       <c r="I66" s="4" t="s">
+        <v>480</v>
+      </c>
+      <c r="J66" s="7" t="s">
         <v>481</v>
       </c>
-      <c r="J66" s="7" t="s">
+      <c r="K66" s="4" t="s">
         <v>482</v>
-      </c>
-      <c r="K66" s="4" t="s">
-        <v>483</v>
       </c>
       <c r="L66" s="4">
         <v>15</v>
@@ -6991,7 +7090,7 @@
         <v>280</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D67" s="4">
         <v>9.9</v>
@@ -7000,7 +7099,7 @@
         <v>209</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>287</v>
@@ -7009,13 +7108,13 @@
         <v>136</v>
       </c>
       <c r="I67" s="4" t="s">
+        <v>485</v>
+      </c>
+      <c r="J67" s="7" t="s">
         <v>486</v>
       </c>
-      <c r="J67" s="7" t="s">
+      <c r="K67" s="4" t="s">
         <v>487</v>
-      </c>
-      <c r="K67" s="4" t="s">
-        <v>488</v>
       </c>
       <c r="L67" s="4">
         <v>15</v>
@@ -7029,7 +7128,7 @@
         <v>280</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D68" s="4">
         <v>9.9</v>
@@ -7038,7 +7137,7 @@
         <v>209</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G68" s="4">
         <v>1</v>
@@ -7047,13 +7146,13 @@
         <v>136</v>
       </c>
       <c r="I68" s="4" t="s">
+        <v>490</v>
+      </c>
+      <c r="J68" s="7" t="s">
         <v>491</v>
       </c>
-      <c r="J68" s="7" t="s">
+      <c r="K68" s="4" t="s">
         <v>492</v>
-      </c>
-      <c r="K68" s="4" t="s">
-        <v>493</v>
       </c>
       <c r="L68" s="4">
         <v>15</v>
@@ -7067,7 +7166,7 @@
         <v>280</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D69" s="4">
         <v>13.4</v>
@@ -7076,22 +7175,22 @@
         <v>319</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="H69" s="4" t="s">
         <v>136</v>
       </c>
       <c r="I69" s="4" t="s">
+        <v>495</v>
+      </c>
+      <c r="J69" s="7" t="s">
         <v>496</v>
       </c>
-      <c r="J69" s="7" t="s">
+      <c r="K69" s="4" t="s">
         <v>497</v>
-      </c>
-      <c r="K69" s="4" t="s">
-        <v>498</v>
       </c>
       <c r="L69" s="4">
         <v>15</v>
@@ -7105,7 +7204,7 @@
         <v>280</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D70" s="4">
         <v>9.4</v>
@@ -7114,22 +7213,22 @@
         <v>172</v>
       </c>
       <c r="F70" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="G70" s="4" t="s">
         <v>500</v>
-      </c>
-      <c r="G70" s="4" t="s">
-        <v>501</v>
       </c>
       <c r="H70" s="4" t="s">
         <v>136</v>
       </c>
       <c r="I70" s="4" t="s">
+        <v>501</v>
+      </c>
+      <c r="J70" s="7" t="s">
         <v>502</v>
       </c>
-      <c r="J70" s="7" t="s">
+      <c r="K70" s="4" t="s">
         <v>503</v>
-      </c>
-      <c r="K70" s="4" t="s">
-        <v>504</v>
       </c>
       <c r="L70" s="4">
         <v>15</v>
@@ -7143,7 +7242,7 @@
         <v>280</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D71" s="4">
         <v>9.9</v>
@@ -7152,22 +7251,22 @@
         <v>172</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="H71" s="4" t="s">
         <v>136</v>
       </c>
       <c r="I71" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="J71" s="7" t="s">
         <v>507</v>
       </c>
-      <c r="J71" s="7" t="s">
+      <c r="K71" s="4" t="s">
         <v>508</v>
-      </c>
-      <c r="K71" s="4" t="s">
-        <v>509</v>
       </c>
       <c r="L71" s="4">
         <v>15</v>
@@ -7181,7 +7280,7 @@
         <v>280</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D72" s="4">
         <v>9.4</v>
@@ -7190,22 +7289,22 @@
         <v>179</v>
       </c>
       <c r="F72" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="G72" s="4" t="s">
         <v>511</v>
-      </c>
-      <c r="G72" s="4" t="s">
-        <v>512</v>
       </c>
       <c r="H72" s="4" t="s">
         <v>136</v>
       </c>
       <c r="I72" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="J72" s="7" t="s">
         <v>513</v>
       </c>
-      <c r="J72" s="7" t="s">
+      <c r="K72" s="4" t="s">
         <v>514</v>
-      </c>
-      <c r="K72" s="4" t="s">
-        <v>515</v>
       </c>
       <c r="L72" s="4">
         <v>15</v>
@@ -7219,7 +7318,7 @@
         <v>280</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D73" s="4">
         <v>9.4</v>
@@ -7228,22 +7327,22 @@
         <v>179</v>
       </c>
       <c r="F73" s="4" t="s">
+        <v>516</v>
+      </c>
+      <c r="G73" s="4" t="s">
         <v>517</v>
-      </c>
-      <c r="G73" s="4" t="s">
-        <v>518</v>
       </c>
       <c r="H73" s="4" t="s">
         <v>136</v>
       </c>
       <c r="I73" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="J73" s="7" t="s">
         <v>519</v>
       </c>
-      <c r="J73" s="7" t="s">
+      <c r="K73" s="4" t="s">
         <v>520</v>
-      </c>
-      <c r="K73" s="4" t="s">
-        <v>521</v>
       </c>
       <c r="L73" s="4">
         <v>15</v>
@@ -7257,7 +7356,7 @@
         <v>131</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D74" s="4">
         <v>13.5</v>
@@ -7266,22 +7365,22 @@
         <v>172</v>
       </c>
       <c r="F74" s="4" t="s">
+        <v>522</v>
+      </c>
+      <c r="G74" s="4" t="s">
         <v>523</v>
-      </c>
-      <c r="G74" s="4" t="s">
-        <v>524</v>
       </c>
       <c r="H74" s="4" t="s">
         <v>136</v>
       </c>
       <c r="I74" s="4" t="s">
+        <v>524</v>
+      </c>
+      <c r="J74" s="7" t="s">
         <v>525</v>
       </c>
-      <c r="J74" s="7" t="s">
+      <c r="K74" s="4" t="s">
         <v>526</v>
-      </c>
-      <c r="K74" s="4" t="s">
-        <v>527</v>
       </c>
       <c r="L74" s="4">
         <v>18</v>
@@ -7295,7 +7394,7 @@
         <v>131</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D75" s="4">
         <v>13.5</v>
@@ -7304,7 +7403,7 @@
         <v>172</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="G75" s="4" t="s">
         <v>344</v>
@@ -7313,13 +7412,13 @@
         <v>136</v>
       </c>
       <c r="I75" s="4" t="s">
+        <v>529</v>
+      </c>
+      <c r="J75" s="7" t="s">
         <v>530</v>
       </c>
-      <c r="J75" s="7" t="s">
+      <c r="K75" s="4" t="s">
         <v>531</v>
-      </c>
-      <c r="K75" s="4" t="s">
-        <v>532</v>
       </c>
       <c r="L75" s="4">
         <v>18</v>
@@ -7333,7 +7432,7 @@
         <v>131</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D76" s="4">
         <v>14.8</v>
@@ -7342,7 +7441,7 @@
         <v>209</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="G76" s="4" t="s">
         <v>344</v>
@@ -7351,13 +7450,13 @@
         <v>136</v>
       </c>
       <c r="I76" s="4" t="s">
+        <v>534</v>
+      </c>
+      <c r="J76" s="7" t="s">
         <v>535</v>
       </c>
-      <c r="J76" s="7" t="s">
+      <c r="K76" s="4" t="s">
         <v>536</v>
-      </c>
-      <c r="K76" s="4" t="s">
-        <v>537</v>
       </c>
       <c r="L76" s="4">
         <v>18</v>
@@ -7371,7 +7470,7 @@
         <v>131</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D77" s="4">
         <v>15.5</v>
@@ -7380,7 +7479,7 @@
         <v>209</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="G77" s="4" t="s">
         <v>344</v>
@@ -7389,13 +7488,13 @@
         <v>136</v>
       </c>
       <c r="I77" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="J77" s="7" t="s">
         <v>540</v>
       </c>
-      <c r="J77" s="7" t="s">
+      <c r="K77" s="4" t="s">
         <v>541</v>
-      </c>
-      <c r="K77" s="4" t="s">
-        <v>542</v>
       </c>
       <c r="L77" s="4">
         <v>18</v>
@@ -7418,22 +7517,22 @@
         <v>209</v>
       </c>
       <c r="F78" s="4" t="s">
+        <v>542</v>
+      </c>
+      <c r="G78" s="4" t="s">
         <v>543</v>
-      </c>
-      <c r="G78" s="4" t="s">
-        <v>544</v>
       </c>
       <c r="H78" s="4" t="s">
         <v>136</v>
       </c>
       <c r="I78" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="J78" s="7" t="s">
         <v>545</v>
       </c>
-      <c r="J78" s="7" t="s">
+      <c r="K78" s="4" t="s">
         <v>546</v>
-      </c>
-      <c r="K78" s="4" t="s">
-        <v>547</v>
       </c>
       <c r="L78" s="4">
         <v>14</v>
@@ -7447,7 +7546,7 @@
         <v>305</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D79" s="4">
         <v>12.9</v>
@@ -7456,7 +7555,7 @@
         <v>209</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="G79" s="4" t="s">
         <v>344</v>
@@ -7465,13 +7564,13 @@
         <v>136</v>
       </c>
       <c r="I79" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="J79" s="7" t="s">
         <v>550</v>
       </c>
-      <c r="J79" s="7" t="s">
+      <c r="K79" s="4" t="s">
         <v>551</v>
-      </c>
-      <c r="K79" s="4" t="s">
-        <v>552</v>
       </c>
       <c r="L79" s="4">
         <v>14</v>
@@ -7485,7 +7584,7 @@
         <v>305</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D80" s="4">
         <v>14.9</v>
@@ -7494,22 +7593,22 @@
         <v>209</v>
       </c>
       <c r="F80" s="4" t="s">
+        <v>553</v>
+      </c>
+      <c r="G80" s="4" t="s">
         <v>554</v>
-      </c>
-      <c r="G80" s="4" t="s">
-        <v>555</v>
       </c>
       <c r="H80" s="4" t="s">
         <v>136</v>
       </c>
       <c r="I80" s="4" t="s">
+        <v>555</v>
+      </c>
+      <c r="J80" s="7" t="s">
         <v>556</v>
       </c>
-      <c r="J80" s="7" t="s">
+      <c r="K80" s="4" t="s">
         <v>557</v>
-      </c>
-      <c r="K80" s="4" t="s">
-        <v>558</v>
       </c>
       <c r="L80" s="4">
         <v>14</v>
@@ -7523,7 +7622,7 @@
         <v>305</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D81" s="4">
         <v>13.9</v>
@@ -7532,7 +7631,7 @@
         <v>209</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="G81" s="4" t="s">
         <v>344</v>
@@ -7541,13 +7640,13 @@
         <v>136</v>
       </c>
       <c r="I81" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="J81" s="7" t="s">
         <v>561</v>
       </c>
-      <c r="J81" s="7" t="s">
+      <c r="K81" s="4" t="s">
         <v>562</v>
-      </c>
-      <c r="K81" s="4" t="s">
-        <v>563</v>
       </c>
       <c r="L81" s="4">
         <v>14</v>
@@ -7561,7 +7660,7 @@
         <v>305</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D82" s="4">
         <v>14.9</v>
@@ -7570,20 +7669,20 @@
         <v>209</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="G82" s="4"/>
       <c r="H82" s="4" t="s">
         <v>136</v>
       </c>
       <c r="I82" s="4" t="s">
+        <v>565</v>
+      </c>
+      <c r="J82" s="7" t="s">
         <v>566</v>
       </c>
-      <c r="J82" s="7" t="s">
+      <c r="K82" s="4" t="s">
         <v>567</v>
-      </c>
-      <c r="K82" s="4" t="s">
-        <v>568</v>
       </c>
       <c r="L82" s="4">
         <v>14</v>
@@ -7597,7 +7696,7 @@
         <v>305</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D83" s="4">
         <v>10.9</v>
@@ -7606,22 +7705,22 @@
         <v>172</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="H83" s="4" t="s">
         <v>136</v>
       </c>
       <c r="I83" s="4" t="s">
+        <v>570</v>
+      </c>
+      <c r="J83" s="7" t="s">
         <v>571</v>
       </c>
-      <c r="J83" s="7" t="s">
+      <c r="K83" s="4" t="s">
         <v>572</v>
-      </c>
-      <c r="K83" s="4" t="s">
-        <v>573</v>
       </c>
       <c r="L83" s="4">
         <v>14</v>
@@ -7635,7 +7734,7 @@
         <v>305</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D84" s="4">
         <v>9.9</v>
@@ -7644,7 +7743,7 @@
         <v>179</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="G84" s="4" t="s">
         <v>355</v>
@@ -7653,13 +7752,13 @@
         <v>136</v>
       </c>
       <c r="I84" s="4" t="s">
+        <v>575</v>
+      </c>
+      <c r="J84" s="7" t="s">
         <v>576</v>
       </c>
-      <c r="J84" s="7" t="s">
+      <c r="K84" s="4" t="s">
         <v>577</v>
-      </c>
-      <c r="K84" s="4" t="s">
-        <v>578</v>
       </c>
       <c r="L84" s="4">
         <v>14</v>
@@ -7673,7 +7772,7 @@
         <v>191</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D85" s="4">
         <v>13.8</v>
@@ -7682,7 +7781,7 @@
         <v>209</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="G85" s="4" t="s">
         <v>344</v>
@@ -7691,13 +7790,13 @@
         <v>136</v>
       </c>
       <c r="I85" s="4" t="s">
+        <v>580</v>
+      </c>
+      <c r="J85" s="7" t="s">
         <v>581</v>
       </c>
-      <c r="J85" s="7" t="s">
+      <c r="K85" s="4" t="s">
         <v>582</v>
-      </c>
-      <c r="K85" s="4" t="s">
-        <v>583</v>
       </c>
       <c r="L85" s="4">
         <v>11</v>
@@ -7711,7 +7810,7 @@
         <v>191</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D86" s="4">
         <v>13.8</v>
@@ -7720,7 +7819,7 @@
         <v>209</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="G86" s="4">
         <v>18</v>
@@ -7729,13 +7828,13 @@
         <v>136</v>
       </c>
       <c r="I86" s="4" t="s">
+        <v>585</v>
+      </c>
+      <c r="J86" s="7" t="s">
         <v>586</v>
       </c>
-      <c r="J86" s="7" t="s">
+      <c r="K86" s="4" t="s">
         <v>587</v>
-      </c>
-      <c r="K86" s="4" t="s">
-        <v>588</v>
       </c>
       <c r="L86" s="4">
         <v>11</v>
@@ -7749,7 +7848,7 @@
         <v>191</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D87" s="4">
         <v>13.5</v>
@@ -7758,7 +7857,7 @@
         <v>172</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="G87" s="4">
         <v>6</v>
@@ -7767,13 +7866,13 @@
         <v>136</v>
       </c>
       <c r="I87" s="4" t="s">
+        <v>590</v>
+      </c>
+      <c r="J87" s="7" t="s">
         <v>591</v>
       </c>
-      <c r="J87" s="7" t="s">
+      <c r="K87" s="4" t="s">
         <v>592</v>
-      </c>
-      <c r="K87" s="4" t="s">
-        <v>593</v>
       </c>
       <c r="L87" s="4">
         <v>11</v>
@@ -7787,7 +7886,7 @@
         <v>191</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D88" s="4">
         <v>12.5</v>
@@ -7796,22 +7895,22 @@
         <v>172</v>
       </c>
       <c r="F88" s="4" t="s">
+        <v>594</v>
+      </c>
+      <c r="G88" s="4" t="s">
         <v>595</v>
-      </c>
-      <c r="G88" s="4" t="s">
-        <v>596</v>
       </c>
       <c r="H88" s="4" t="s">
         <v>136</v>
       </c>
       <c r="I88" s="4" t="s">
+        <v>596</v>
+      </c>
+      <c r="J88" s="7" t="s">
         <v>597</v>
       </c>
-      <c r="J88" s="7" t="s">
+      <c r="K88" s="4" t="s">
         <v>598</v>
-      </c>
-      <c r="K88" s="4" t="s">
-        <v>599</v>
       </c>
       <c r="L88" s="4">
         <v>11</v>
@@ -7825,7 +7924,7 @@
         <v>191</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D89" s="4">
         <v>13.5</v>
@@ -7834,22 +7933,22 @@
         <v>172</v>
       </c>
       <c r="F89" s="4" t="s">
+        <v>600</v>
+      </c>
+      <c r="G89" s="4" t="s">
         <v>601</v>
-      </c>
-      <c r="G89" s="4" t="s">
-        <v>602</v>
       </c>
       <c r="H89" s="4" t="s">
         <v>136</v>
       </c>
       <c r="I89" s="4" t="s">
+        <v>602</v>
+      </c>
+      <c r="J89" s="7" t="s">
         <v>603</v>
       </c>
-      <c r="J89" s="7" t="s">
+      <c r="K89" s="4" t="s">
         <v>604</v>
-      </c>
-      <c r="K89" s="4" t="s">
-        <v>605</v>
       </c>
       <c r="L89" s="4">
         <v>11</v>
@@ -7863,7 +7962,7 @@
         <v>191</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D90" s="4">
         <v>13.8</v>
@@ -7872,22 +7971,22 @@
         <v>319</v>
       </c>
       <c r="F90" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="G90" s="4" t="s">
         <v>607</v>
-      </c>
-      <c r="G90" s="4" t="s">
-        <v>608</v>
       </c>
       <c r="H90" s="4" t="s">
         <v>136</v>
       </c>
       <c r="I90" s="4" t="s">
+        <v>608</v>
+      </c>
+      <c r="J90" s="7" t="s">
         <v>609</v>
       </c>
-      <c r="J90" s="7" t="s">
+      <c r="K90" s="4" t="s">
         <v>610</v>
-      </c>
-      <c r="K90" s="4" t="s">
-        <v>611</v>
       </c>
       <c r="L90" s="4">
         <v>11</v>
@@ -7901,7 +8000,7 @@
         <v>191</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D91" s="4">
         <v>13.8</v>
@@ -7910,22 +8009,22 @@
         <v>319</v>
       </c>
       <c r="F91" s="4" t="s">
+        <v>612</v>
+      </c>
+      <c r="G91" s="4" t="s">
         <v>613</v>
-      </c>
-      <c r="G91" s="4" t="s">
-        <v>614</v>
       </c>
       <c r="H91" s="4" t="s">
         <v>136</v>
       </c>
       <c r="I91" s="4" t="s">
+        <v>614</v>
+      </c>
+      <c r="J91" s="7" t="s">
         <v>615</v>
       </c>
-      <c r="J91" s="7" t="s">
+      <c r="K91" s="4" t="s">
         <v>616</v>
-      </c>
-      <c r="K91" s="4" t="s">
-        <v>617</v>
       </c>
       <c r="L91" s="4">
         <v>11</v>
@@ -7939,7 +8038,7 @@
         <v>191</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D92" s="4">
         <v>12.5</v>
@@ -7948,22 +8047,22 @@
         <v>209</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="G92" s="4" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="H92" s="4" t="s">
         <v>136</v>
       </c>
       <c r="I92" s="4" t="s">
+        <v>619</v>
+      </c>
+      <c r="J92" s="7" t="s">
         <v>620</v>
       </c>
-      <c r="J92" s="7" t="s">
+      <c r="K92" s="4" t="s">
         <v>621</v>
-      </c>
-      <c r="K92" s="4" t="s">
-        <v>622</v>
       </c>
       <c r="L92" s="4">
         <v>11</v>
@@ -7977,7 +8076,7 @@
         <v>191</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D93" s="4">
         <v>13.8</v>
@@ -7986,20 +8085,20 @@
         <v>209</v>
       </c>
       <c r="F93" s="4" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="G93" s="4"/>
       <c r="H93" s="4" t="s">
         <v>136</v>
       </c>
       <c r="I93" s="4" t="s">
+        <v>624</v>
+      </c>
+      <c r="J93" s="7" t="s">
         <v>625</v>
       </c>
-      <c r="J93" s="7" t="s">
+      <c r="K93" s="4" t="s">
         <v>626</v>
-      </c>
-      <c r="K93" s="4" t="s">
-        <v>627</v>
       </c>
       <c r="L93" s="4">
         <v>11</v>
@@ -8013,7 +8112,7 @@
         <v>305</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="D94" s="4">
         <v>6.8</v>
@@ -8022,20 +8121,20 @@
         <v>209</v>
       </c>
       <c r="F94" s="4" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="G94" s="4"/>
       <c r="H94" s="4" t="s">
         <v>136</v>
       </c>
       <c r="I94" s="4" t="s">
+        <v>629</v>
+      </c>
+      <c r="J94" s="7" t="s">
         <v>630</v>
       </c>
-      <c r="J94" s="7" t="s">
+      <c r="K94" s="4" t="s">
         <v>631</v>
-      </c>
-      <c r="K94" s="4" t="s">
-        <v>632</v>
       </c>
       <c r="L94" s="4">
         <v>13</v>
@@ -8049,7 +8148,7 @@
         <v>305</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D95" s="4">
         <v>7.9</v>
@@ -8058,7 +8157,7 @@
         <v>209</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="G95" s="4" t="s">
         <v>344</v>
@@ -8067,13 +8166,13 @@
         <v>136</v>
       </c>
       <c r="I95" s="4" t="s">
+        <v>634</v>
+      </c>
+      <c r="J95" s="7" t="s">
         <v>635</v>
       </c>
-      <c r="J95" s="7" t="s">
+      <c r="K95" s="4" t="s">
         <v>636</v>
-      </c>
-      <c r="K95" s="4" t="s">
-        <v>637</v>
       </c>
       <c r="L95" s="4">
         <v>13</v>
@@ -8087,7 +8186,7 @@
         <v>305</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D96" s="4">
         <v>7.4</v>
@@ -8096,22 +8195,22 @@
         <v>209</v>
       </c>
       <c r="F96" s="4" t="s">
+        <v>638</v>
+      </c>
+      <c r="G96" s="4" t="s">
         <v>639</v>
-      </c>
-      <c r="G96" s="4" t="s">
-        <v>640</v>
       </c>
       <c r="H96" s="4" t="s">
         <v>136</v>
       </c>
       <c r="I96" s="4" t="s">
+        <v>640</v>
+      </c>
+      <c r="J96" s="7" t="s">
         <v>641</v>
       </c>
-      <c r="J96" s="7" t="s">
+      <c r="K96" s="4" t="s">
         <v>642</v>
-      </c>
-      <c r="K96" s="4" t="s">
-        <v>643</v>
       </c>
       <c r="L96" s="4">
         <v>13</v>
@@ -8125,7 +8224,7 @@
         <v>305</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D97" s="4">
         <v>6.9</v>
@@ -8134,7 +8233,7 @@
         <v>172</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="G97" s="4">
         <v>1</v>
@@ -8143,13 +8242,13 @@
         <v>136</v>
       </c>
       <c r="I97" s="4" t="s">
+        <v>645</v>
+      </c>
+      <c r="J97" s="7" t="s">
         <v>646</v>
       </c>
-      <c r="J97" s="7" t="s">
+      <c r="K97" s="4" t="s">
         <v>647</v>
-      </c>
-      <c r="K97" s="4" t="s">
-        <v>648</v>
       </c>
       <c r="L97" s="4">
         <v>13</v>
@@ -8163,7 +8262,7 @@
         <v>305</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D98" s="4">
         <v>7.2</v>
@@ -8172,20 +8271,20 @@
         <v>172</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="G98" s="4"/>
       <c r="H98" s="4" t="s">
         <v>136</v>
       </c>
       <c r="I98" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="J98" s="7" t="s">
         <v>651</v>
       </c>
-      <c r="J98" s="7" t="s">
+      <c r="K98" s="4" t="s">
         <v>652</v>
-      </c>
-      <c r="K98" s="4" t="s">
-        <v>653</v>
       </c>
       <c r="L98" s="4">
         <v>13</v>
@@ -8199,7 +8298,7 @@
         <v>305</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D99" s="4">
         <v>8.5</v>
@@ -8208,7 +8307,7 @@
         <v>319</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="G99" s="4">
         <v>4</v>
@@ -8217,13 +8316,13 @@
         <v>136</v>
       </c>
       <c r="I99" s="4" t="s">
+        <v>655</v>
+      </c>
+      <c r="J99" s="7" t="s">
         <v>656</v>
       </c>
-      <c r="J99" s="7" t="s">
+      <c r="K99" s="4" t="s">
         <v>657</v>
-      </c>
-      <c r="K99" s="4" t="s">
-        <v>658</v>
       </c>
       <c r="L99" s="4">
         <v>13</v>
@@ -8237,7 +8336,7 @@
         <v>305</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="D100" s="4">
         <v>9.9</v>
@@ -8246,7 +8345,7 @@
         <v>319</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="G100" s="4">
         <v>15</v>
@@ -8255,13 +8354,13 @@
         <v>136</v>
       </c>
       <c r="I100" s="4" t="s">
+        <v>660</v>
+      </c>
+      <c r="J100" s="7" t="s">
         <v>661</v>
       </c>
-      <c r="J100" s="7" t="s">
+      <c r="K100" s="4" t="s">
         <v>662</v>
-      </c>
-      <c r="K100" s="4" t="s">
-        <v>663</v>
       </c>
       <c r="L100" s="4">
         <v>13</v>
@@ -8275,7 +8374,7 @@
         <v>305</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D101" s="4">
         <v>8.9</v>
@@ -8284,22 +8383,22 @@
         <v>319</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="G101" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="H101" s="4" t="s">
         <v>136</v>
       </c>
       <c r="I101" s="4" t="s">
+        <v>664</v>
+      </c>
+      <c r="J101" s="7" t="s">
         <v>665</v>
       </c>
-      <c r="J101" s="7" t="s">
+      <c r="K101" s="4" t="s">
         <v>666</v>
-      </c>
-      <c r="K101" s="4" t="s">
-        <v>667</v>
       </c>
       <c r="L101" s="4">
         <v>13</v>
@@ -8441,10 +8540,175 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF4D624E-8E28-784A-BEC7-768DBD17C5A3}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView zoomScale="171" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="19.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="32.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="42.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="3" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>862</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>865</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>866</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>863</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>871</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D14" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC55C975-5D1C-6E41-9916-C5BD900D32CB}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView zoomScale="171" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="18.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="3" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>860</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>861</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>864</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BA84880-E797-490C-B6C8-7F8FA112873A}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
@@ -8458,7 +8722,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>122</v>
@@ -8478,16 +8742,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C2">
         <v>3.2</v>
       </c>
       <c r="D2" t="s">
+        <v>672</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>673</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8495,16 +8759,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="C3">
         <v>3.2</v>
       </c>
       <c r="D3" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8512,16 +8776,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="C4">
         <v>3.2</v>
       </c>
       <c r="D4" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8529,16 +8793,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C5">
         <v>3.2</v>
       </c>
       <c r="D5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8546,16 +8810,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="C6">
         <v>3.8</v>
       </c>
       <c r="D6" t="s">
+        <v>681</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>682</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8563,16 +8827,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C7">
         <v>3.8</v>
       </c>
       <c r="D7" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8580,16 +8844,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="C8">
         <v>3.8</v>
       </c>
       <c r="D8" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8597,16 +8861,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C9">
         <v>2.8</v>
       </c>
       <c r="D9" t="s">
+        <v>688</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>689</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8614,16 +8878,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C10">
         <v>3.2</v>
       </c>
       <c r="D10" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8631,16 +8895,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C11">
         <v>3.3</v>
       </c>
       <c r="D11" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8648,16 +8912,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8665,16 +8929,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C13">
         <v>3.4</v>
       </c>
       <c r="D13" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8682,16 +8946,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C14">
         <v>2.2000000000000002</v>
       </c>
       <c r="D14" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8699,16 +8963,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C15">
         <v>2.2000000000000002</v>
       </c>
       <c r="D15" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8716,16 +8980,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="C16">
         <v>2.2000000000000002</v>
       </c>
       <c r="D16" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8733,16 +8997,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C17">
         <v>3.6</v>
       </c>
       <c r="D17" t="s">
+        <v>705</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>706</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>707</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8750,16 +9014,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="C18">
         <v>3.4</v>
       </c>
       <c r="D18" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8767,16 +9031,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C19">
         <v>3.4</v>
       </c>
       <c r="D19" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8784,16 +9048,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="C20">
         <v>8</v>
       </c>
       <c r="D20" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8801,16 +9065,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="C21">
         <v>3.8</v>
       </c>
       <c r="D21" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8818,16 +9082,16 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C22">
         <v>3.6</v>
       </c>
       <c r="D22" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8835,16 +9099,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C23">
         <v>3.6</v>
       </c>
       <c r="D23" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8852,16 +9116,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="C24">
         <v>2.4</v>
       </c>
       <c r="D24" t="s">
+        <v>719</v>
+      </c>
+      <c r="E24" s="7" t="s">
         <v>720</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>721</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -8869,16 +9133,16 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="C25">
         <v>2.2000000000000002</v>
       </c>
       <c r="D25" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -8886,16 +9150,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C26">
         <v>2.2000000000000002</v>
       </c>
       <c r="D26" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -8903,16 +9167,16 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C27">
         <v>3.2</v>
       </c>
       <c r="D27" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -8920,16 +9184,16 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="C28">
         <v>3.2</v>
       </c>
       <c r="D28" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -8937,16 +9201,16 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C29">
         <v>3.8</v>
       </c>
       <c r="D29" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="128" x14ac:dyDescent="0.2">
@@ -8954,16 +9218,16 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C30">
         <v>3.8</v>
       </c>
       <c r="D30" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="64" x14ac:dyDescent="0.2">
@@ -8971,16 +9235,16 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C31">
         <v>3.8</v>
       </c>
       <c r="D31" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="64" x14ac:dyDescent="0.2">
@@ -8988,16 +9252,16 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C32">
         <v>4.5</v>
       </c>
       <c r="D32" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -9005,16 +9269,16 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="C33">
         <v>4.5</v>
       </c>
       <c r="D33" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -9022,16 +9286,16 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="C34">
         <v>4.5</v>
       </c>
       <c r="D34" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -9039,16 +9303,16 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C35">
         <v>5.5</v>
       </c>
       <c r="D35" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -9056,16 +9320,16 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C36">
         <v>5.5</v>
       </c>
       <c r="D36" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="64" x14ac:dyDescent="0.2">
@@ -9073,16 +9337,16 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="C37">
         <v>4.5</v>
       </c>
       <c r="D37" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -9090,16 +9354,16 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C38">
         <v>5.5</v>
       </c>
       <c r="D38" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -9107,16 +9371,16 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C39">
         <v>3.4</v>
       </c>
       <c r="D39" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -9124,16 +9388,16 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="C40">
         <v>3.2</v>
       </c>
       <c r="D40" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="64" x14ac:dyDescent="0.2">
@@ -9141,16 +9405,16 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="C41">
         <v>2.8</v>
       </c>
       <c r="D41" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="80" x14ac:dyDescent="0.2">
@@ -9158,16 +9422,16 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="C42">
         <v>8</v>
       </c>
       <c r="D42" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="80" x14ac:dyDescent="0.2">
@@ -9175,16 +9439,16 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="C43">
         <v>8</v>
       </c>
       <c r="D43" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="128" x14ac:dyDescent="0.2">
@@ -9192,16 +9456,16 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C44">
         <v>8</v>
       </c>
       <c r="D44" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -9209,16 +9473,16 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C45">
         <v>4</v>
       </c>
       <c r="D45" t="s">
+        <v>762</v>
+      </c>
+      <c r="E45" s="7" t="s">
         <v>763</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>764</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -9226,16 +9490,16 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C46">
         <v>4</v>
       </c>
       <c r="D46" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -9243,16 +9507,16 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="C47">
         <v>4</v>
       </c>
       <c r="D47" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="64" x14ac:dyDescent="0.2">
@@ -9260,16 +9524,16 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="C48">
         <v>4</v>
       </c>
       <c r="D48" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -9277,16 +9541,16 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="C49">
         <v>4</v>
       </c>
       <c r="D49" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="64" x14ac:dyDescent="0.2">
@@ -9294,16 +9558,16 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C50">
         <v>4</v>
       </c>
       <c r="D50" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -9311,16 +9575,16 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="C51">
         <v>4</v>
       </c>
       <c r="D51" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -9328,16 +9592,16 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C52">
         <v>3.8</v>
       </c>
       <c r="D52" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
   </sheetData>
@@ -9401,11 +9665,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA5374C0-011E-45E4-BE95-3545615AB94A}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="157" workbookViewId="0">
       <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
@@ -9418,7 +9682,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>125</v>
@@ -9429,7 +9693,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -9437,7 +9701,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -9445,7 +9709,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -9453,7 +9717,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -9461,7 +9725,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -9469,7 +9733,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -9477,7 +9741,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -9485,7 +9749,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -9493,7 +9757,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -9501,7 +9765,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E11" s="9"/>
     </row>
@@ -9510,7 +9774,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -9518,7 +9782,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -9526,7 +9790,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -9534,7 +9798,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -9542,7 +9806,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -9550,7 +9814,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -9558,7 +9822,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -9566,7 +9830,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -9574,7 +9838,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -9582,7 +9846,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -9590,7 +9854,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -9598,7 +9862,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -9606,7 +9870,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -9614,7 +9878,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -9622,7 +9886,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -9630,7 +9894,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -9638,7 +9902,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -9646,7 +9910,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -9654,7 +9918,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -9662,7 +9926,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -9670,7 +9934,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -9678,7 +9942,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -9686,7 +9950,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -9694,7 +9958,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -9702,7 +9966,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -9710,7 +9974,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -9718,7 +9982,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -9726,7 +9990,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -9734,7 +9998,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -9742,7 +10006,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -9750,7 +10014,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -9758,7 +10022,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -9766,7 +10030,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -9774,7 +10038,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -9782,7 +10046,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -9790,7 +10054,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -9798,7 +10062,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -9806,7 +10070,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
   </sheetData>
@@ -9817,11 +10081,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7676E93-61D2-C540-86CA-3A4648138FB3}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="168" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -9834,10 +10098,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>827</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>828</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>829</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>3</v>
@@ -9848,10 +10112,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>830</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>831</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -9859,10 +10123,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>831</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>832</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>833</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -9870,7 +10134,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -9888,7 +10152,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C6" s="3"/>
     </row>
@@ -9897,10 +10161,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>835</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>836</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>837</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -9908,7 +10172,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C8" s="3"/>
     </row>
@@ -9917,10 +10181,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>838</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>839</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>840</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -9928,7 +10192,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="C10" s="3"/>
     </row>
@@ -9937,7 +10201,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="C11" s="3"/>
     </row>
@@ -9946,7 +10210,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="C12" s="3"/>
     </row>
@@ -9955,10 +10219,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>843</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>844</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>845</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -9966,10 +10230,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -9977,10 +10241,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>846</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>847</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>848</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -9988,10 +10252,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>848</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>849</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>850</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -9999,7 +10263,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="C17" s="3"/>
     </row>
@@ -10008,7 +10272,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="C18" s="3"/>
     </row>
@@ -10017,10 +10281,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>852</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>853</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>854</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -10047,46 +10311,55 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6AE945D-A4BC-40F9-9C14-6D890D7EBEAD}">
-  <dimension ref="A2:A9"/>
+  <dimension ref="A2:C9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView zoomScale="223" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="40.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>859</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+        <v>858</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
+        <v>667</v>
+      </c>
+      <c r="C3" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
         <v>668</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-    </row>
-    <row r="5" spans="1:1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-    </row>
-    <row r="7" spans="1:1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
     </row>
   </sheetData>
@@ -10094,7 +10367,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5BD8ED7-FA83-431A-B318-CB16642876F8}">
   <dimension ref="A1:E1"/>
   <sheetViews>
@@ -10112,16 +10385,16 @@
         <v>122</v>
       </c>
       <c r="B1" t="s">
+        <v>854</v>
+      </c>
+      <c r="C1" t="s">
         <v>855</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>856</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>857</v>
-      </c>
-      <c r="E1" t="s">
-        <v>858</v>
       </c>
     </row>
   </sheetData>

</xml_diff>